<commit_message>
Adicionado arquivo de configuração "chocolate"
</commit_message>
<xml_diff>
--- a/sniper/tools/results_multicore-8_splash2.xlsx
+++ b/sniper/tools/results_multicore-8_splash2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Runtime</t>
   </si>
@@ -34,13 +34,13 @@
     <t>Average Bandwidth Usage</t>
   </si>
   <si>
+    <t>Max Checkpoint Size</t>
+  </si>
+  <si>
     <t>Number of Checkpoints</t>
   </si>
   <si>
     <t>Error</t>
-  </si>
-  <si>
-    <t>baseline-nvm</t>
   </si>
   <si>
     <t>donuts-lor</t>
@@ -500,68 +500,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="1"/>
+      <c r="P1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="S1" s="1"/>
-      <c r="T1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" spans="1:25">
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -570,16 +566,16 @@
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
@@ -588,16 +584,16 @@
         <v>10</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>9</v>
@@ -605,99 +601,66 @@
       <c r="S2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:19">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>105345382</v>
+        <v>107887892</v>
       </c>
       <c r="C4">
-        <v>107887892</v>
+        <v>107638902</v>
       </c>
       <c r="D4">
-        <v>107638902</v>
+        <v>316639</v>
       </c>
       <c r="E4">
-        <v>238199</v>
+        <v>306167</v>
       </c>
       <c r="F4">
-        <v>316639</v>
+        <v>115826</v>
       </c>
       <c r="G4">
-        <v>306167</v>
+        <v>106599</v>
       </c>
       <c r="H4">
-        <v>65380</v>
+        <v>200813</v>
       </c>
       <c r="I4">
-        <v>115826</v>
+        <v>106599</v>
       </c>
       <c r="J4">
-        <v>106599</v>
+        <v>3149</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1676</v>
       </c>
       <c r="L4">
-        <v>200813</v>
+        <v>0.02</v>
       </c>
       <c r="M4">
-        <v>106599</v>
+        <v>0.02</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2803904</v>
       </c>
       <c r="O4">
-        <v>3149</v>
+        <v>786496</v>
       </c>
       <c r="P4">
-        <v>1676</v>
+        <v>23</v>
       </c>
       <c r="Q4">
-        <v>0.02</v>
-      </c>
-      <c r="R4">
-        <v>0.02</v>
-      </c>
-      <c r="S4">
-        <v>0.02</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>23</v>
-      </c>
-      <c r="V4">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -749,168 +712,120 @@
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="R5" t="s">
         <v>41</v>
       </c>
-      <c r="X5" t="s">
+      <c r="S5" t="s">
         <v>41</v>
       </c>
-      <c r="Y5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>53878986</v>
+        <v>57285497</v>
       </c>
       <c r="C6">
-        <v>57285497</v>
+        <v>56662157</v>
       </c>
       <c r="D6">
-        <v>56662157</v>
+        <v>807614</v>
       </c>
       <c r="E6">
-        <v>641086</v>
+        <v>813947</v>
       </c>
       <c r="F6">
-        <v>807614</v>
+        <v>419050</v>
       </c>
       <c r="G6">
-        <v>813947</v>
+        <v>432582</v>
       </c>
       <c r="H6">
-        <v>263096</v>
+        <v>388564</v>
       </c>
       <c r="I6">
-        <v>419050</v>
+        <v>432582</v>
       </c>
       <c r="J6">
-        <v>432582</v>
+        <v>6100</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>6793</v>
       </c>
       <c r="L6">
-        <v>388564</v>
+        <v>0.14</v>
       </c>
       <c r="M6">
-        <v>432582</v>
+        <v>0.14</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2926912</v>
       </c>
       <c r="O6">
-        <v>6100</v>
+        <v>1365312</v>
       </c>
       <c r="P6">
-        <v>6793</v>
+        <v>55</v>
       </c>
       <c r="Q6">
-        <v>0.11</v>
-      </c>
-      <c r="R6">
-        <v>0.14</v>
-      </c>
-      <c r="S6">
-        <v>0.14</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>55</v>
-      </c>
-      <c r="V6">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:19">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>95359555</v>
+        <v>102561765</v>
       </c>
       <c r="C7">
-        <v>102561765</v>
+        <v>101011165</v>
       </c>
       <c r="D7">
-        <v>101011165</v>
+        <v>3277092</v>
       </c>
       <c r="E7">
-        <v>3120890</v>
+        <v>3252064</v>
       </c>
       <c r="F7">
-        <v>3277092</v>
+        <v>1088335</v>
       </c>
       <c r="G7">
-        <v>3252064</v>
+        <v>1102040</v>
       </c>
       <c r="H7">
-        <v>1023571</v>
+        <v>2188757</v>
       </c>
       <c r="I7">
-        <v>1088335</v>
+        <v>1102040</v>
       </c>
       <c r="J7">
-        <v>1102040</v>
+        <v>34292</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>17325</v>
       </c>
       <c r="L7">
-        <v>2188757</v>
+        <v>0.31</v>
       </c>
       <c r="M7">
-        <v>1102040</v>
+        <v>0.32</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>3009536</v>
       </c>
       <c r="O7">
-        <v>34292</v>
+        <v>1250688</v>
       </c>
       <c r="P7">
-        <v>17325</v>
+        <v>194</v>
       </c>
       <c r="Q7">
-        <v>0.32</v>
-      </c>
-      <c r="R7">
-        <v>0.31</v>
-      </c>
-      <c r="S7">
-        <v>0.32</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>194</v>
-      </c>
-      <c r="V7">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:19">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -962,440 +877,332 @@
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="R8" t="s">
         <v>41</v>
       </c>
-      <c r="X8" t="s">
+      <c r="S8" t="s">
         <v>41</v>
       </c>
-      <c r="Y8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9">
-        <v>143888555</v>
+        <v>150518965</v>
       </c>
       <c r="C9">
-        <v>150518965</v>
+        <v>149852765</v>
       </c>
       <c r="D9">
-        <v>149852765</v>
+        <v>3436591</v>
       </c>
       <c r="E9">
-        <v>3894214</v>
+        <v>3444488</v>
       </c>
       <c r="F9">
-        <v>3436591</v>
+        <v>653750</v>
       </c>
       <c r="G9">
-        <v>3444488</v>
+        <v>663309</v>
       </c>
       <c r="H9">
-        <v>1121271</v>
+        <v>2782841</v>
       </c>
       <c r="I9">
-        <v>653750</v>
+        <v>663309</v>
       </c>
       <c r="J9">
-        <v>663309</v>
+        <v>43561</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>10453</v>
       </c>
       <c r="L9">
-        <v>2782841</v>
+        <v>0.22</v>
       </c>
       <c r="M9">
-        <v>663309</v>
+        <v>0.23</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>102083392</v>
       </c>
       <c r="O9">
-        <v>43561</v>
+        <v>1488640</v>
       </c>
       <c r="P9">
-        <v>10453</v>
+        <v>159</v>
       </c>
       <c r="Q9">
-        <v>0.27</v>
-      </c>
-      <c r="R9">
-        <v>0.22</v>
-      </c>
-      <c r="S9">
-        <v>0.23</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>159</v>
-      </c>
-      <c r="V9">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10">
-        <v>87278223</v>
+        <v>92830587</v>
       </c>
       <c r="C10">
-        <v>92830587</v>
+        <v>92557280</v>
       </c>
       <c r="D10">
-        <v>92557280</v>
+        <v>2992853</v>
       </c>
       <c r="E10">
-        <v>2860150</v>
+        <v>2992460</v>
       </c>
       <c r="F10">
-        <v>2992853</v>
+        <v>1018043</v>
       </c>
       <c r="G10">
-        <v>2992460</v>
+        <v>1014163</v>
       </c>
       <c r="H10">
-        <v>938585</v>
+        <v>1974810</v>
       </c>
       <c r="I10">
-        <v>1018043</v>
+        <v>1014163</v>
       </c>
       <c r="J10">
-        <v>1014163</v>
+        <v>30957</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>15940</v>
       </c>
       <c r="L10">
-        <v>1974810</v>
+        <v>0.32</v>
       </c>
       <c r="M10">
-        <v>1014163</v>
+        <v>0.32</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>2930304</v>
       </c>
       <c r="O10">
-        <v>30957</v>
+        <v>1319744</v>
       </c>
       <c r="P10">
-        <v>15940</v>
+        <v>188</v>
       </c>
       <c r="Q10">
-        <v>0.32</v>
-      </c>
-      <c r="R10">
-        <v>0.32</v>
-      </c>
-      <c r="S10">
-        <v>0.32</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
         <v>188</v>
       </c>
-      <c r="V10">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11">
-        <v>92128355</v>
+        <v>96409365</v>
       </c>
       <c r="C11">
-        <v>96409365</v>
+        <v>96647965</v>
       </c>
       <c r="D11">
-        <v>96647965</v>
+        <v>3005831</v>
       </c>
       <c r="E11">
-        <v>2900692</v>
+        <v>3017174</v>
       </c>
       <c r="F11">
-        <v>3005831</v>
+        <v>1029403</v>
       </c>
       <c r="G11">
-        <v>3017174</v>
+        <v>1022289</v>
       </c>
       <c r="H11">
-        <v>952672</v>
+        <v>1976428</v>
       </c>
       <c r="I11">
-        <v>1029403</v>
+        <v>1022289</v>
       </c>
       <c r="J11">
-        <v>1022289</v>
+        <v>30989</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>16074</v>
       </c>
       <c r="L11">
-        <v>1976428</v>
+        <v>0.31</v>
       </c>
       <c r="M11">
-        <v>1022289</v>
+        <v>0.31</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>2526144</v>
       </c>
       <c r="O11">
-        <v>30989</v>
+        <v>1353728</v>
       </c>
       <c r="P11">
-        <v>16074</v>
+        <v>198</v>
       </c>
       <c r="Q11">
-        <v>0.31</v>
-      </c>
-      <c r="R11">
-        <v>0.31</v>
-      </c>
-      <c r="S11">
-        <v>0.31</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>198</v>
-      </c>
-      <c r="V11">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:19">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>94971155</v>
+        <v>100576365</v>
       </c>
       <c r="C12">
-        <v>100576365</v>
+        <v>100348965</v>
       </c>
       <c r="D12">
-        <v>100348965</v>
+        <v>3246806</v>
       </c>
       <c r="E12">
-        <v>3105935</v>
+        <v>3248514</v>
       </c>
       <c r="F12">
-        <v>3246806</v>
+        <v>1103412</v>
       </c>
       <c r="G12">
-        <v>3248514</v>
+        <v>1107430</v>
       </c>
       <c r="H12">
-        <v>1016578</v>
+        <v>2143394</v>
       </c>
       <c r="I12">
-        <v>1103412</v>
+        <v>1107430</v>
       </c>
       <c r="J12">
-        <v>1107430</v>
+        <v>33592</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>17412</v>
       </c>
       <c r="L12">
-        <v>2143394</v>
+        <v>0.32</v>
       </c>
       <c r="M12">
-        <v>1107430</v>
+        <v>0.32</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>2681408</v>
       </c>
       <c r="O12">
-        <v>33592</v>
+        <v>1290944</v>
       </c>
       <c r="P12">
-        <v>17412</v>
+        <v>204</v>
       </c>
       <c r="Q12">
-        <v>0.32</v>
-      </c>
-      <c r="R12">
-        <v>0.32</v>
-      </c>
-      <c r="S12">
-        <v>0.32</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>204</v>
-      </c>
-      <c r="V12">
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B13">
-        <v>95054155</v>
+        <v>101073565</v>
       </c>
       <c r="C13">
-        <v>101073565</v>
+        <v>100963165</v>
       </c>
       <c r="D13">
-        <v>100963165</v>
+        <v>3252788</v>
       </c>
       <c r="E13">
-        <v>3118411</v>
+        <v>3252622</v>
       </c>
       <c r="F13">
-        <v>3252788</v>
+        <v>1101693</v>
       </c>
       <c r="G13">
-        <v>3252622</v>
+        <v>1093589</v>
       </c>
       <c r="H13">
-        <v>1023018</v>
+        <v>2151095</v>
       </c>
       <c r="I13">
-        <v>1101693</v>
+        <v>1093589</v>
       </c>
       <c r="J13">
-        <v>1093589</v>
+        <v>33717</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>17189</v>
       </c>
       <c r="L13">
-        <v>2151095</v>
+        <v>0.32</v>
       </c>
       <c r="M13">
-        <v>1093589</v>
+        <v>0.32</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>2871808</v>
       </c>
       <c r="O13">
-        <v>33717</v>
+        <v>1276992</v>
       </c>
       <c r="P13">
-        <v>17189</v>
+        <v>210</v>
       </c>
       <c r="Q13">
-        <v>0.32</v>
-      </c>
-      <c r="R13">
-        <v>0.32</v>
-      </c>
-      <c r="S13">
-        <v>0.32</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>210</v>
-      </c>
-      <c r="V13">
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B14">
-        <v>95169955</v>
+        <v>101166165</v>
       </c>
       <c r="C14">
-        <v>101166165</v>
+        <v>100943365</v>
       </c>
       <c r="D14">
-        <v>100943365</v>
+        <v>3250416</v>
       </c>
       <c r="E14">
-        <v>3116096</v>
+        <v>3254963</v>
       </c>
       <c r="F14">
-        <v>3250416</v>
+        <v>1099486</v>
       </c>
       <c r="G14">
-        <v>3254963</v>
+        <v>1101363</v>
       </c>
       <c r="H14">
-        <v>1021358</v>
+        <v>2150930</v>
       </c>
       <c r="I14">
-        <v>1099486</v>
+        <v>1101363</v>
       </c>
       <c r="J14">
-        <v>1101363</v>
+        <v>33717</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>17309</v>
       </c>
       <c r="L14">
-        <v>2150930</v>
+        <v>0.32</v>
       </c>
       <c r="M14">
-        <v>1101363</v>
+        <v>0.32</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>2679744</v>
       </c>
       <c r="O14">
-        <v>33717</v>
+        <v>1375744</v>
       </c>
       <c r="P14">
-        <v>17309</v>
+        <v>208</v>
       </c>
       <c r="Q14">
-        <v>0.32</v>
-      </c>
-      <c r="R14">
-        <v>0.32</v>
-      </c>
-      <c r="S14">
-        <v>0.32</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>208</v>
-      </c>
-      <c r="V14">
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1447,32 +1254,14 @@
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="R15" t="s">
         <v>42</v>
       </c>
-      <c r="X15" t="s">
+      <c r="S15" t="s">
         <v>42</v>
       </c>
-      <c r="Y15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1524,100 +1313,67 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16" t="s">
+      <c r="R16" t="s">
         <v>41</v>
       </c>
-      <c r="X16" t="s">
+      <c r="S16" t="s">
         <v>41</v>
       </c>
-      <c r="Y16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B17">
-        <v>67805868</v>
+        <v>76655040</v>
       </c>
       <c r="C17">
-        <v>76655040</v>
+        <v>76438756</v>
       </c>
       <c r="D17">
-        <v>76438756</v>
+        <v>1441781</v>
       </c>
       <c r="E17">
-        <v>1376221</v>
+        <v>1437013</v>
       </c>
       <c r="F17">
-        <v>1441781</v>
+        <v>687879</v>
       </c>
       <c r="G17">
-        <v>1437013</v>
+        <v>685836</v>
       </c>
       <c r="H17">
-        <v>646190</v>
+        <v>753902</v>
       </c>
       <c r="I17">
-        <v>687879</v>
+        <v>685836</v>
       </c>
       <c r="J17">
-        <v>685836</v>
+        <v>11816</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>10754</v>
       </c>
       <c r="L17">
-        <v>753902</v>
+        <v>0.18</v>
       </c>
       <c r="M17">
-        <v>685836</v>
+        <v>0.18</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>5126208</v>
       </c>
       <c r="O17">
-        <v>11816</v>
+        <v>1390464</v>
       </c>
       <c r="P17">
-        <v>10754</v>
+        <v>73</v>
       </c>
       <c r="Q17">
-        <v>0.2</v>
-      </c>
-      <c r="R17">
-        <v>0.18</v>
-      </c>
-      <c r="S17">
-        <v>0.18</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
         <v>73</v>
       </c>
-      <c r="V17">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1669,100 +1425,67 @@
       <c r="Q18">
         <v>0</v>
       </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18" t="s">
+      <c r="R18" t="s">
         <v>41</v>
       </c>
-      <c r="X18" t="s">
+      <c r="S18" t="s">
         <v>41</v>
       </c>
-      <c r="Y18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25">
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B19">
-        <v>77639946</v>
+        <v>93108356</v>
       </c>
       <c r="C19">
-        <v>93108356</v>
+        <v>93011156</v>
       </c>
       <c r="D19">
-        <v>93011156</v>
+        <v>1864461</v>
       </c>
       <c r="E19">
-        <v>1584731</v>
+        <v>1863595</v>
       </c>
       <c r="F19">
-        <v>1864461</v>
+        <v>774594</v>
       </c>
       <c r="G19">
-        <v>1863595</v>
+        <v>774647</v>
       </c>
       <c r="H19">
-        <v>694029</v>
+        <v>1089867</v>
       </c>
       <c r="I19">
-        <v>774594</v>
+        <v>774647</v>
       </c>
       <c r="J19">
-        <v>774647</v>
+        <v>17913</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>12942</v>
       </c>
       <c r="L19">
-        <v>1089867</v>
+        <v>0.2</v>
       </c>
       <c r="M19">
-        <v>774647</v>
+        <v>0.2</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>4286016</v>
       </c>
       <c r="O19">
-        <v>17913</v>
+        <v>812544</v>
       </c>
       <c r="P19">
-        <v>12942</v>
+        <v>1642</v>
       </c>
       <c r="Q19">
-        <v>0.2</v>
-      </c>
-      <c r="R19">
-        <v>0.2</v>
-      </c>
-      <c r="S19">
-        <v>0.2</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>1642</v>
-      </c>
-      <c r="V19">
         <v>1630</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1814,100 +1537,67 @@
       <c r="Q20">
         <v>0</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="R20" t="s">
         <v>41</v>
       </c>
-      <c r="X20" t="s">
+      <c r="S20" t="s">
         <v>41</v>
       </c>
-      <c r="Y20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B21">
-        <v>291959161</v>
+        <v>332150403</v>
       </c>
       <c r="C21">
-        <v>332150403</v>
+        <v>329849602</v>
       </c>
       <c r="D21">
-        <v>329849602</v>
+        <v>18770684</v>
       </c>
       <c r="E21">
-        <v>18505703</v>
+        <v>18696668</v>
       </c>
       <c r="F21">
-        <v>18770684</v>
+        <v>5200708</v>
       </c>
       <c r="G21">
-        <v>18696668</v>
+        <v>5279381</v>
       </c>
       <c r="H21">
-        <v>5077464</v>
+        <v>13569976</v>
       </c>
       <c r="I21">
-        <v>5200708</v>
+        <v>5279381</v>
       </c>
       <c r="J21">
-        <v>5279381</v>
+        <v>212329</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>82767</v>
       </c>
       <c r="L21">
-        <v>13569976</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="M21">
-        <v>5279381</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>7915648</v>
       </c>
       <c r="O21">
-        <v>212329</v>
+        <v>1422912</v>
       </c>
       <c r="P21">
-        <v>82767</v>
+        <v>570</v>
       </c>
       <c r="Q21">
-        <v>0.63</v>
-      </c>
-      <c r="R21">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="S21">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>570</v>
-      </c>
-      <c r="V21">
         <v>551</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:19">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1959,236 +1649,173 @@
       <c r="Q22">
         <v>0</v>
       </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22" t="s">
+      <c r="R22" t="s">
         <v>41</v>
       </c>
-      <c r="X22" t="s">
+      <c r="S22" t="s">
         <v>41</v>
       </c>
-      <c r="Y22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B23">
-        <v>340036938</v>
+        <v>392130793</v>
       </c>
       <c r="C23">
-        <v>392130793</v>
+        <v>388815339</v>
       </c>
       <c r="D23">
-        <v>388815339</v>
+        <v>19849096</v>
       </c>
       <c r="E23">
-        <v>18973198</v>
+        <v>20599344</v>
       </c>
       <c r="F23">
-        <v>19849096</v>
+        <v>5745054</v>
       </c>
       <c r="G23">
-        <v>20599344</v>
+        <v>5764654</v>
       </c>
       <c r="H23">
-        <v>5117080</v>
+        <v>14104042</v>
       </c>
       <c r="I23">
-        <v>5745054</v>
+        <v>5764654</v>
       </c>
       <c r="J23">
-        <v>5764654</v>
+        <v>220774</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>90536</v>
       </c>
       <c r="L23">
-        <v>14104042</v>
+        <v>0.5</v>
       </c>
       <c r="M23">
-        <v>5764654</v>
+        <v>0.53</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>4977280</v>
       </c>
       <c r="O23">
-        <v>220774</v>
+        <v>1427584</v>
       </c>
       <c r="P23">
-        <v>90536</v>
+        <v>806</v>
       </c>
       <c r="Q23">
-        <v>0.55</v>
-      </c>
-      <c r="R23">
-        <v>0.5</v>
-      </c>
-      <c r="S23">
-        <v>0.53</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>806</v>
-      </c>
-      <c r="V23">
         <v>921</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24">
-        <v>83410120</v>
+        <v>84363718</v>
       </c>
       <c r="C24">
-        <v>84363718</v>
+        <v>84539727</v>
       </c>
       <c r="D24">
-        <v>84539727</v>
+        <v>46848</v>
       </c>
       <c r="E24">
-        <v>39065</v>
+        <v>53911</v>
       </c>
       <c r="F24">
-        <v>46848</v>
+        <v>18418</v>
       </c>
       <c r="G24">
-        <v>53911</v>
+        <v>25516</v>
       </c>
       <c r="H24">
-        <v>14271</v>
+        <v>28430</v>
       </c>
       <c r="I24">
-        <v>18418</v>
+        <v>25516</v>
       </c>
       <c r="J24">
-        <v>25516</v>
+        <v>447</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>402</v>
       </c>
       <c r="L24">
-        <v>28430</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>25516</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>786624</v>
       </c>
       <c r="O24">
-        <v>447</v>
+        <v>898880</v>
       </c>
       <c r="P24">
-        <v>402</v>
+        <v>3</v>
       </c>
       <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>3</v>
-      </c>
-      <c r="V24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:19">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B25">
-        <v>58090300</v>
+        <v>59116900</v>
       </c>
       <c r="C25">
-        <v>59116900</v>
+        <v>58952500</v>
       </c>
       <c r="D25">
-        <v>58952500</v>
+        <v>329939</v>
       </c>
       <c r="E25">
-        <v>278278</v>
+        <v>340366</v>
       </c>
       <c r="F25">
-        <v>329939</v>
+        <v>140958</v>
       </c>
       <c r="G25">
-        <v>340366</v>
+        <v>150905</v>
       </c>
       <c r="H25">
-        <v>87091</v>
+        <v>188981</v>
       </c>
       <c r="I25">
-        <v>140958</v>
+        <v>150905</v>
       </c>
       <c r="J25">
-        <v>150905</v>
+        <v>2970</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>2376</v>
       </c>
       <c r="L25">
-        <v>188981</v>
+        <v>0.05</v>
       </c>
       <c r="M25">
-        <v>150905</v>
+        <v>0.05</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>2048896</v>
       </c>
       <c r="O25">
-        <v>2970</v>
+        <v>700416</v>
       </c>
       <c r="P25">
-        <v>2376</v>
+        <v>32</v>
       </c>
       <c r="Q25">
-        <v>0.04</v>
-      </c>
-      <c r="R25">
-        <v>0.05</v>
-      </c>
-      <c r="S25">
-        <v>0.05</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>32</v>
-      </c>
-      <c r="V25">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:19">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -2240,168 +1867,120 @@
       <c r="Q26">
         <v>0</v>
       </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26" t="s">
+      <c r="R26" t="s">
         <v>41</v>
       </c>
-      <c r="X26" t="s">
+      <c r="S26" t="s">
         <v>41</v>
       </c>
-      <c r="Y26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B27">
-        <v>88638721</v>
+        <v>90729525</v>
       </c>
       <c r="C27">
-        <v>90729525</v>
+        <v>90065925</v>
       </c>
       <c r="D27">
-        <v>90065925</v>
+        <v>281987</v>
       </c>
       <c r="E27">
-        <v>248426</v>
+        <v>269541</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>35</v>
+      </c>
+      <c r="H27">
         <v>281987</v>
       </c>
-      <c r="G27">
-        <v>269541</v>
-      </c>
-      <c r="H27">
-        <v>17284</v>
-      </c>
       <c r="I27">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J27">
-        <v>35</v>
+        <v>4406</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27">
-        <v>281987</v>
+        <v>0.03</v>
       </c>
       <c r="M27">
-        <v>35</v>
+        <v>0.02</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>11117824</v>
       </c>
       <c r="O27">
-        <v>4406</v>
+        <v>1250432</v>
       </c>
       <c r="P27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27">
-        <v>0.02</v>
-      </c>
-      <c r="R27">
-        <v>0.03</v>
-      </c>
-      <c r="S27">
-        <v>0.02</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B28">
-        <v>85601121</v>
+        <v>87010125</v>
       </c>
       <c r="C28">
-        <v>87010125</v>
+        <v>86337925</v>
       </c>
       <c r="D28">
-        <v>86337925</v>
+        <v>300813</v>
       </c>
       <c r="E28">
-        <v>263091</v>
+        <v>283037</v>
       </c>
       <c r="F28">
-        <v>300813</v>
+        <v>10321</v>
       </c>
       <c r="G28">
-        <v>283037</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>17932</v>
+        <v>290492</v>
       </c>
       <c r="I28">
-        <v>10321</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>4540</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>290492</v>
+        <v>0.03</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>11099712</v>
       </c>
       <c r="O28">
-        <v>4540</v>
+        <v>1226560</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28">
-        <v>0.03</v>
-      </c>
-      <c r="R28">
-        <v>0.03</v>
-      </c>
-      <c r="S28">
-        <v>0.03</v>
-      </c>
-      <c r="T28">
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-      <c r="V28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -2453,100 +2032,67 @@
       <c r="Q29">
         <v>0</v>
       </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="W29" t="s">
+      <c r="R29" t="s">
         <v>42</v>
       </c>
-      <c r="X29" t="s">
+      <c r="S29" t="s">
         <v>42</v>
       </c>
-      <c r="Y29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B30">
-        <v>53814307</v>
+        <v>54351766</v>
       </c>
       <c r="C30">
-        <v>54351766</v>
+        <v>54431562</v>
       </c>
       <c r="D30">
-        <v>54431562</v>
+        <v>283215</v>
       </c>
       <c r="E30">
-        <v>231169</v>
+        <v>282126</v>
       </c>
       <c r="F30">
-        <v>283215</v>
+        <v>141791</v>
       </c>
       <c r="G30">
-        <v>282126</v>
+        <v>141721</v>
       </c>
       <c r="H30">
-        <v>97164</v>
+        <v>141424</v>
       </c>
       <c r="I30">
-        <v>141791</v>
+        <v>141721</v>
       </c>
       <c r="J30">
-        <v>141721</v>
+        <v>2370</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>2379</v>
       </c>
       <c r="L30">
-        <v>141424</v>
+        <v>0.05</v>
       </c>
       <c r="M30">
-        <v>141721</v>
+        <v>0.05</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>114496</v>
       </c>
       <c r="O30">
-        <v>2370</v>
+        <v>47936</v>
       </c>
       <c r="P30">
-        <v>2379</v>
+        <v>329</v>
       </c>
       <c r="Q30">
-        <v>0.04</v>
-      </c>
-      <c r="R30">
-        <v>0.05</v>
-      </c>
-      <c r="S30">
-        <v>0.05</v>
-      </c>
-      <c r="T30">
-        <v>0</v>
-      </c>
-      <c r="U30">
         <v>329</v>
       </c>
-      <c r="V30">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -2598,109 +2144,77 @@
       <c r="Q31">
         <v>0</v>
       </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-      <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="W31" t="s">
+      <c r="R31" t="s">
         <v>41</v>
       </c>
-      <c r="X31" t="s">
+      <c r="S31" t="s">
         <v>41</v>
       </c>
-      <c r="Y31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B32">
-        <v>81376368</v>
+        <v>82716441</v>
       </c>
       <c r="C32">
-        <v>82716441</v>
+        <v>82814666</v>
       </c>
       <c r="D32">
-        <v>82814666</v>
+        <v>437502</v>
       </c>
       <c r="E32">
-        <v>404940</v>
+        <v>435171</v>
       </c>
       <c r="F32">
-        <v>437502</v>
+        <v>53419</v>
       </c>
       <c r="G32">
-        <v>435171</v>
+        <v>53510</v>
       </c>
       <c r="H32">
-        <v>50896</v>
+        <v>384083</v>
       </c>
       <c r="I32">
-        <v>53419</v>
+        <v>53510</v>
       </c>
       <c r="J32">
-        <v>53510</v>
+        <v>6039</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>873</v>
       </c>
       <c r="L32">
-        <v>384083</v>
+        <v>0.05</v>
       </c>
       <c r="M32">
-        <v>53510</v>
+        <v>0.05</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>2309568</v>
       </c>
       <c r="O32">
-        <v>6039</v>
+        <v>174656</v>
       </c>
       <c r="P32">
-        <v>873</v>
+        <v>76</v>
       </c>
       <c r="Q32">
-        <v>0.04</v>
-      </c>
-      <c r="R32">
-        <v>0.05</v>
-      </c>
-      <c r="S32">
-        <v>0.05</v>
-      </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>76</v>
-      </c>
-      <c r="V32">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
+  <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>